<commit_message>
adding CVPIA to keyword set
</commit_message>
<xml_diff>
--- a/data-raw/metadata/2022_update/F4F2021_metadata2022.xlsx
+++ b/data-raw/metadata/2022_update/F4F2021_metadata2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/CVPIA/edi.996.1/data-raw/metadata/2022_update/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92669B68-C6FD-5D4B-92F0-D70B73D6D2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E88E8D-C8E9-B440-AB68-780398D54BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="500" windowWidth="28000" windowHeight="15940" tabRatio="543" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="800" yWindow="500" windowWidth="28000" windowHeight="15760" tabRatio="543" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="personnel" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="298">
   <si>
     <t>first_name</t>
   </si>
@@ -933,6 +933,9 @@
   </si>
   <si>
     <t>Fish Food on Floodplain Farm Fields 2019, 2021, and 2022</t>
+  </si>
+  <si>
+    <t>CVPIA</t>
   </si>
 </sst>
 </file>
@@ -1517,7 +1520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1551,10 +1554,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1745,6 +1748,11 @@
       </c>
       <c r="B23" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>